<commit_message>
Edit of Risk Management
</commit_message>
<xml_diff>
--- a/Projectmanagement/Risk Management.xlsx
+++ b/Projectmanagement/Risk Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\DH\TrackYourFit\TrackYourFit_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\DH\TrackYourFit\TrackYourFit_docs\Projectmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B4A32C-391D-4118-9DCF-791261D55994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA16DC0B-2DA8-4001-B4CC-23EAF6200627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="5660" windowWidth="19390" windowHeight="11350" xr2:uid="{165AA583-885E-40B6-9C75-B7FB8F56993D}"/>
+    <workbookView xWindow="11430" yWindow="7140" windowWidth="19390" windowHeight="11350" xr2:uid="{165AA583-885E-40B6-9C75-B7FB8F56993D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Risk Name</t>
   </si>
@@ -47,19 +47,28 @@
     <t>Risk Impact</t>
   </si>
   <si>
-    <t>Risk Factor</t>
-  </si>
-  <si>
     <t>1 to 10</t>
   </si>
   <si>
     <t>1 to 100</t>
   </si>
   <si>
-    <t>not enought time</t>
-  </si>
-  <si>
-    <t>…</t>
+    <t>Not enought time</t>
+  </si>
+  <si>
+    <t>Underestimated complexity</t>
+  </si>
+  <si>
+    <t>Risk response strategy</t>
+  </si>
+  <si>
+    <t>Unreliability of a team member</t>
+  </si>
+  <si>
+    <t>A team member doesnt complete his work.</t>
+  </si>
+  <si>
+    <t>The other team member have to plit up the undone work and complete it.</t>
   </si>
 </sst>
 </file>
@@ -111,12 +120,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -431,30 +445,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE69595-5EB9-4243-A58D-1EEBF09B9C02}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.90625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
     <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -470,20 +481,66 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4">
+        <v>0.4</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 13: Risk Management and time spend per use case
</commit_message>
<xml_diff>
--- a/Projectmanagement/Risk Management.xlsx
+++ b/Projectmanagement/Risk Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\DH\TrackYourFit\TrackYourFit_docs\Projectmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA16DC0B-2DA8-4001-B4CC-23EAF6200627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4779A9-0F47-4068-AD9A-1E8767A71AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="7140" windowWidth="19390" windowHeight="11350" xr2:uid="{165AA583-885E-40B6-9C75-B7FB8F56993D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{165AA583-885E-40B6-9C75-B7FB8F56993D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Risk Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Underestimated complexity</t>
   </si>
   <si>
-    <t>Risk response strategy</t>
-  </si>
-  <si>
     <t>Unreliability of a team member</t>
   </si>
   <si>
@@ -69,13 +66,88 @@
   </si>
   <si>
     <t>The other team member have to plit up the undone work and complete it.</t>
+  </si>
+  <si>
+    <t>Not finishing our scope of this semester</t>
+  </si>
+  <si>
+    <t>Wrong Priorities</t>
+  </si>
+  <si>
+    <t>The set goals are too hard to achive</t>
+  </si>
+  <si>
+    <t>Risk migration</t>
+  </si>
+  <si>
+    <t>Self-reflections and changes when sprints are not completed.</t>
+  </si>
+  <si>
+    <t>Lose of team members</t>
+  </si>
+  <si>
+    <t>Losing a team member (e.g. due to failing the exams)</t>
+  </si>
+  <si>
+    <t>Not focusing on the scope.</t>
+  </si>
+  <si>
+    <t>Not getting carried away by smaller, less needed tasks.</t>
+  </si>
+  <si>
+    <t>Coronavirus</t>
+  </si>
+  <si>
+    <t>Unexpected circumstances (e.g. internet failing, serverhosting platforms not available)</t>
+  </si>
+  <si>
+    <t>Self hosting of a server, other than that there is nothing we could do.</t>
+  </si>
+  <si>
+    <t>Careful planning of the sprints.</t>
+  </si>
+  <si>
+    <t>Everybody should have knoeledge about the whole code.</t>
+  </si>
+  <si>
+    <t>Dataloss</t>
+  </si>
+  <si>
+    <t>Loss through a github mistake or error.</t>
+  </si>
+  <si>
+    <t>Careful git handling.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Risk factor</t>
+  </si>
+  <si>
+    <t>Person in charge of tracking</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Toni Einecker</t>
+  </si>
+  <si>
+    <t>Janis Fix</t>
+  </si>
+  <si>
+    <t>Tobias Bühler</t>
+  </si>
+  <si>
+    <t>Johannes Zipfel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +157,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,8 +196,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -129,13 +209,140 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -146,6 +353,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADEA53D8-7C10-49CB-89DB-8C24248C9873}" name="Tabelle1" displayName="Tabelle1" ref="B3:I10" totalsRowShown="0" headerRowBorderDxfId="7">
+  <autoFilter ref="B3:I10" xr:uid="{2DBBD95F-2792-4A6A-9F89-DF8D50B9A84E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I10">
+    <sortCondition descending="1" ref="G3:G10"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8D886E79-1B18-4D72-AC20-B69DCF5355EE}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{34302095-110E-4946-A3C3-EE16945EAC5A}" name="Risk Name"/>
+    <tableColumn id="3" xr3:uid="{618C9FA2-62AE-483A-A796-56CE63E3F6EA}" name="Risk Description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{B933F5FB-AA93-4C7F-8DDD-749BAC9D3555}" name="Risk Probability of Occurrence " dataDxfId="5" dataCellStyle="Prozent"/>
+    <tableColumn id="5" xr3:uid="{1AE36974-6113-4801-8693-B4A55CF8D0FF}" name="Risk Impact"/>
+    <tableColumn id="6" xr3:uid="{B1403537-C19A-4A2D-AB34-36FA4408D005}" name="Risk factor">
+      <calculatedColumnFormula>E4*F4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{CCCCBDED-4541-407E-8B1C-F297AEC370A3}" name="Risk migration" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{F3FA53F1-02BB-4E53-B82A-E8E179FDFF97}" name="Person in charge of tracking"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,105 +674,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE69595-5EB9-4243-A58D-1EEBF09B9C02}">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
-    <col min="6" max="6" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" customWidth="1"/>
+    <col min="6" max="7" width="11.36328125" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <f>E5*F5</f>
+        <v>2.4499999999999997</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f>E6*F6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="F7">
         <v>8</v>
       </c>
+      <c r="G7">
+        <f>E7*F7</f>
+        <v>1.2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="8" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <f>E8*F8</f>
+        <v>1.05</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9">
         <v>6</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f>E9*F9</f>
         <v>0.4</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E5">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F10">
         <v>5</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="3"/>
+      <c r="G10">
+        <f>E10*F10</f>
+        <v>0.25</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F4:G10">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>3.5</formula>
+      <formula>7.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>3.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>7.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>